<commit_message>
List participants to excel
</commit_message>
<xml_diff>
--- a/output/MagnusL.xlsx
+++ b/output/MagnusL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744BD535-5BD3-46E6-BDBD-09B703D47318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35B176D-10F4-4552-9F20-35026CFD61D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="5400" yWindow="2138" windowWidth="16200" windowHeight="9397" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="43080" yWindow="780" windowWidth="29040" windowHeight="17640" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Klasser" sheetId="2" r:id="rId1"/>
@@ -425,11 +425,11 @@
   </x:cellStyleXfs>
   <x:cellXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="top" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment vertical="top" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <x:alignment horizontal="left" vertical="top" wrapText="1"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -755,13 +755,13 @@
   <x:sheetPr codeName="Sheet2">
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:O6"/>
+  <x:dimension ref="A1:O1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D12" sqref="D12"/>
+    <x:sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+      <x:selection activeCell="B10" sqref="B10"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="10.308281" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <x:sheetFormatPr defaultColWidth="13.8425" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <x:sheetData>
     <x:row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <x:c r="A1" s="3" t="s">
@@ -810,180 +810,150 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:15" customFormat="1" ht="19.15" customHeight="1" x14ac:dyDescent="0.45">
-      <x:c r="A2" s="4" t="n">
+    <x:row r="2" spans="1:15">
+      <x:c r="A2" s="0" t="n">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B2" s="4" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C2" s="4" t="n">
+      <x:c r="C2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D2" s="4" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E2" s="4" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="F2" s="4" t="s"/>
-      <x:c r="G2" s="4" t="s"/>
-      <x:c r="H2" s="4" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="I2" s="4" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="J2" s="4" t="s"/>
-      <x:c r="K2" s="4" t="s"/>
-      <x:c r="L2" s="4" t="s">
+      <x:c r="L2" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="M2" s="4" t="s">
+      <x:c r="M2" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="N2" s="4" t="s"/>
-      <x:c r="O2" s="4" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:15" customFormat="1" ht="19.15" customHeight="1" x14ac:dyDescent="0.45">
-      <x:c r="A3" s="4" t="n">
+    </x:row>
+    <x:row r="3" spans="1:15">
+      <x:c r="A3" s="0" t="n">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B3" s="4" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C3" s="4" t="n">
+      <x:c r="C3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D3" s="4" t="s">
+      <x:c r="D3" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E3" s="4" t="s">
+      <x:c r="E3" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="F3" s="4" t="s"/>
-      <x:c r="G3" s="4" t="s"/>
-      <x:c r="H3" s="4" t="s">
+      <x:c r="H3" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="I3" s="4" t="s">
+      <x:c r="I3" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="J3" s="4" t="s"/>
-      <x:c r="K3" s="4" t="s"/>
-      <x:c r="L3" s="4" t="s">
+      <x:c r="L3" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="M3" s="4" t="s">
+      <x:c r="M3" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="N3" s="4" t="s"/>
-      <x:c r="O3" s="4" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:15" customFormat="1" ht="19.15" customHeight="1" x14ac:dyDescent="0.45">
-      <x:c r="A4" s="4" t="n">
+    </x:row>
+    <x:row r="4" spans="1:15">
+      <x:c r="A4" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B4" s="4" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C4" s="4" t="n">
+      <x:c r="C4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D4" s="4" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E4" s="4" t="s">
+      <x:c r="E4" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="F4" s="4" t="s"/>
-      <x:c r="G4" s="4" t="s"/>
-      <x:c r="H4" s="4" t="s">
+      <x:c r="H4" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="I4" s="4" t="s">
+      <x:c r="I4" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="J4" s="4" t="s"/>
-      <x:c r="K4" s="4" t="s"/>
-      <x:c r="L4" s="4" t="s">
+      <x:c r="L4" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="M4" s="4" t="s">
+      <x:c r="M4" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="N4" s="4" t="s"/>
-      <x:c r="O4" s="4" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:15" customFormat="1" ht="19.15" customHeight="1" x14ac:dyDescent="0.45">
-      <x:c r="A5" s="4" t="n">
+    </x:row>
+    <x:row r="5" spans="1:15">
+      <x:c r="A5" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B5" s="4" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C5" s="4" t="n">
+      <x:c r="C5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D5" s="4" t="s">
+      <x:c r="D5" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E5" s="4" t="s">
+      <x:c r="E5" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="F5" s="4" t="s"/>
-      <x:c r="G5" s="4" t="s"/>
-      <x:c r="H5" s="4" t="s">
+      <x:c r="H5" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="I5" s="4" t="s">
+      <x:c r="I5" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="J5" s="4" t="s"/>
-      <x:c r="K5" s="4" t="s"/>
-      <x:c r="L5" s="4" t="s">
+      <x:c r="L5" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="M5" s="4" t="s">
+      <x:c r="M5" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="N5" s="4" t="s"/>
-      <x:c r="O5" s="4" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:15" customFormat="1" ht="19.15" customHeight="1" x14ac:dyDescent="0.45">
-      <x:c r="A6" s="4" t="n">
+    </x:row>
+    <x:row r="6" spans="1:15">
+      <x:c r="A6" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B6" s="4" t="s">
+      <x:c r="B6" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C6" s="4" t="n">
+      <x:c r="C6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D6" s="4" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E6" s="4" t="s">
+      <x:c r="E6" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="F6" s="4" t="s"/>
-      <x:c r="G6" s="4" t="s"/>
-      <x:c r="H6" s="4" t="s">
+      <x:c r="H6" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="I6" s="4" t="s">
+      <x:c r="I6" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="J6" s="4" t="s"/>
-      <x:c r="K6" s="4" t="s"/>
-      <x:c r="L6" s="4" t="s">
+      <x:c r="L6" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="M6" s="4" t="s">
+      <x:c r="M6" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="N6" s="4" t="s"/>
-      <x:c r="O6" s="4" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>